<commit_message>
Added logging and move file functionality
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -42,17 +42,23 @@
     <t>PriceAuditFolder</t>
   </si>
   <si>
-    <t>Price Audit Folder</t>
-  </si>
-  <si>
-    <t>Processed Price Audit Data</t>
+    <t>\\compass-usa\cgcorp\AccountingServices\Secure\Systems and Projects\Systems\SAP\Projects\UiPath\FB Dev\PriceAudits\Detail.5.9.2019.SC\Loaded\Processed</t>
+  </si>
+  <si>
+    <t>\\compass-usa\cgcorp\AccountingServices\Secure\Systems and Projects\Systems\SAP\Projects\UiPath\FB Dev\PriceAudits\Detail.5.9.2019.SC\Loaded\Loaded</t>
+  </si>
+  <si>
+    <t>TemplateFile</t>
+  </si>
+  <si>
+    <t>\\compass-usa\cgcorp\AccountingServices\Secure\Systems and Projects\Systems\SAP\Projects\UiPath\FB Dev\PriceAudits\Template\02 February 2019-DiCarlo Distributors Template.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +70,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,14 +100,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,15 +389,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="64.28515625" customWidth="1"/>
+    <col min="1" max="1" width="64.28515625" customWidth="1"/>
+    <col min="2" max="2" width="148.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -398,8 +417,8 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -409,15 +428,28 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Try/Catch to handle error files and move them to specified ErrorFolder. (Change location of ErrorFolder in the Data\Config.xlsx file)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>\\compass-usa\cgcorp\AccountingServices\Secure\Systems and Projects\Systems\SAP\Projects\UiPath\FB Dev\PriceAudits\Template\02 February 2019-DiCarlo Distributors Template.xlsx</t>
+  </si>
+  <si>
+    <t>ErrorFolder</t>
+  </si>
+  <si>
+    <t>\\compass-usa\cgcorp\AccountingServices\Secure\Systems and Projects\Systems\SAP\Projects\UiPath\FB Dev\PriceAudits\Detail.5.9.2019.SC\Loaded\Errors</t>
+  </si>
+  <si>
+    <t>Template where headers are pulled from.</t>
+  </si>
+  <si>
+    <t>Where files are moved if there is an error reading or processing them.</t>
   </si>
 </sst>
 </file>
@@ -389,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,14 +454,29 @@
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Configured VBA coding to format columns to fit text
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -69,10 +69,25 @@
     <t>ConsolidatedFile</t>
   </si>
   <si>
-    <t>\\compass-usa\cgcorp\AccountingServices\Secure\Systems and Projects\Systems\SAP\Projects\UiPath\FB Dev\PriceAudits\Detail.5.9.2019.SC\Loaded\PriceAudit_Consolidated.xlsx</t>
-  </si>
-  <si>
     <t>Consolidated price audit file</t>
+  </si>
+  <si>
+    <t>FaultyRowsFile</t>
+  </si>
+  <si>
+    <t>Faulty rows from files with partially correct information</t>
+  </si>
+  <si>
+    <t>\\compass-usa\cgcorp\AccountingServices\Secure\Systems and Projects\Systems\SAP\Projects\UiPath\FB Dev\PriceAudits\Detail.5.9.2019.SC\Loaded\Errors\FaultyRows.xlsm</t>
+  </si>
+  <si>
+    <t>\\compass-usa\cgcorp\AccountingServices\Secure\Systems and Projects\Systems\SAP\Projects\UiPath\FB Dev\PriceAudits\Detail.5.9.2019.SC\Loaded\PriceAudit_Consolidated.xlsm</t>
+  </si>
+  <si>
+    <t>Macros</t>
+  </si>
+  <si>
+    <t>\\compass-usa\cgcorp\AccountingServices\Secure\Systems and Projects\Systems\SAP\Projects\UiPath\Macros</t>
   </si>
 </sst>
 </file>
@@ -410,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O5:O6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,10 +498,29 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -496,8 +530,10 @@
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>